<commit_message>
added country code field and changed profile page design
</commit_message>
<xml_diff>
--- a/public/assests/Drivers.xlsx
+++ b/public/assests/Drivers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Office\Live Project\GaurdianLinkAdmin\public\assests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97401BD-E44D-4DDF-BF85-4B3D006C68E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DBF2C7-8DE1-4BC7-9C02-94E6A4923EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>email</t>
   </si>
@@ -39,12 +39,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
     <t>driver1@example.com</t>
   </si>
   <si>
@@ -91,6 +85,18 @@
   </si>
   <si>
     <t>&lt;company_name&gt;</t>
+  </si>
+  <si>
+    <t>mobile_no_country_code</t>
+  </si>
+  <si>
+    <t>id_no</t>
+  </si>
+  <si>
+    <t>+27</t>
+  </si>
+  <si>
+    <t>mobile_no</t>
   </si>
 </sst>
 </file>
@@ -117,18 +123,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,8 +151,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,10 +372,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M1000"/>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -384,18 +384,19 @@
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.6640625" style="2"/>
+    <col min="5" max="5" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,76 +410,82 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>123</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1">
         <v>7894561230</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1">
         <v>3</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="2">
+        <v>362220</v>
+      </c>
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="2">
-        <v>362220</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -487,8 +494,9 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -497,8 +505,9 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -507,8 +516,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -517,16 +527,17 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>